<commit_message>
Updated documentation for R4 queries.
</commit_message>
<xml_diff>
--- a/documents/eCR_R1.1_FHIR_Mapping_R4_v2.xlsx
+++ b/documents/eCR_R1.1_FHIR_Mapping_R4_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbashyam/git/eCRNow/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B49D36-7E9E-D449-BA00-FFD11F802B14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21713F77-3DAB-A04F-9E89-1D795DA4CAF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="2300" windowWidth="26460" windowHeight="17500" activeTab="1" xr2:uid="{0236C1A8-3996-47BC-AEF5-83819174BBEE}"/>
+    <workbookView xWindow="180" yWindow="2300" windowWidth="32720" windowHeight="18660" activeTab="1" xr2:uid="{0236C1A8-3996-47BC-AEF5-83819174BBEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Queries" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="388">
   <si>
     <t>Data Element</t>
   </si>
@@ -433,11 +433,6 @@
   <si>
     <t>Observation.value
 Observation.component.value</t>
-  </si>
-  <si>
-    <t>GET [base]/Observation?patient=[id]&amp;category=laboratory
-GET [base]/Observation?patient=[id]&amp;code=[LOINC{,LOINC2,LOINC3,...}]
-GET [base]/Observation?patient=[id]&amp;category=laboratory&amp;date=[date]{&amp;date=[date]}</t>
   </si>
   <si>
     <t>ClinicalDocument/recordTarget/patientRole/patient/administrativeGenderCode</t>
@@ -1061,9 +1056,6 @@
     <t>Immunization.practitioner</t>
   </si>
   <si>
-    <t>us-core-observationresults</t>
-  </si>
-  <si>
     <t>registered -&gt; active
 preliminary -&gt; active
 final -&gt; completed
@@ -1259,6 +1251,16 @@
   </si>
   <si>
     <t>Condition</t>
+  </si>
+  <si>
+    <t>GET /MedicationAdministration?patient=[id] or GET /MedicationRequest?patient=[id] 
+or GET /MedicationStatement?patient=[id]</t>
+  </si>
+  <si>
+    <t>us-core-observation-lab</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=[id]&amp;category=LAB</t>
   </si>
 </sst>
 </file>
@@ -1796,8 +1798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1F3ACE-59C5-436A-8107-2305AC5D6F77}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="53.33203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1823,7 +1825,7 @@
         <v>94</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1831,13 +1833,13 @@
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1845,16 +1847,16 @@
         <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -1862,13 +1864,13 @@
         <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -1876,43 +1878,43 @@
         <v>76</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>385</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -1925,10 +1927,10 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
+      <selection pane="bottomRight" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1962,7 +1964,7 @@
         <v>64</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>119</v>
@@ -1983,7 +1985,7 @@
         <v>49</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -1994,7 +1996,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>50</v>
@@ -2019,7 +2021,7 @@
         <v>112</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -2027,13 +2029,13 @@
         <v>100</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>297</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>81</v>
@@ -2055,7 +2057,7 @@
         <v>112</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -2063,13 +2065,13 @@
         <v>100</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>93</v>
@@ -2091,7 +2093,7 @@
         <v>112</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -2099,13 +2101,13 @@
         <v>100</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>93</v>
@@ -2127,18 +2129,18 @@
         <v>112</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>67</v>
@@ -2148,7 +2150,7 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>84</v>
@@ -2160,21 +2162,21 @@
         <v>82</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>68</v>
@@ -2184,7 +2186,7 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>83</v>
@@ -2196,21 +2198,21 @@
         <v>82</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>69</v>
@@ -2220,7 +2222,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>85</v>
@@ -2230,21 +2232,21 @@
         <v>92</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>70</v>
@@ -2254,7 +2256,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>85</v>
@@ -2264,31 +2266,31 @@
         <v>92</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>92</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>86</v>
@@ -2300,21 +2302,21 @@
         <v>82</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>71</v>
@@ -2324,7 +2326,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>87</v>
@@ -2334,21 +2336,21 @@
         <v>92</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>72</v>
@@ -2358,7 +2360,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>87</v>
@@ -2368,21 +2370,21 @@
         <v>92</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>73</v>
@@ -2392,7 +2394,7 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>89</v>
@@ -2402,21 +2404,21 @@
         <v>92</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>74</v>
@@ -2424,7 +2426,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="6"/>
       <c r="G14" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>90</v>
@@ -2436,24 +2438,24 @@
         <v>93</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="4" customFormat="1" ht="65" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>120</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>81</v>
@@ -2462,7 +2464,7 @@
         <v>123</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>121</v>
@@ -2474,21 +2476,21 @@
         <v>81</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>126</v>
@@ -2498,33 +2500,33 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>306</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>307</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>91</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>127</v>
@@ -2534,10 +2536,10 @@
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>91</v>
@@ -2546,21 +2548,21 @@
         <v>92</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>124</v>
@@ -2570,10 +2572,10 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>91</v>
@@ -2582,21 +2584,21 @@
         <v>93</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>125</v>
@@ -2606,10 +2608,10 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>91</v>
@@ -2618,31 +2620,31 @@
         <v>92</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>88</v>
@@ -2654,91 +2656,91 @@
         <v>92</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>51</v>
@@ -2748,31 +2750,31 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>52</v>
@@ -2780,31 +2782,31 @@
       <c r="E24" s="9"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>53</v>
@@ -2812,31 +2814,31 @@
       <c r="E25" s="9"/>
       <c r="F25" s="6"/>
       <c r="G25" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>54</v>
@@ -2844,31 +2846,31 @@
       <c r="E26" s="9"/>
       <c r="F26" s="6"/>
       <c r="G26" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>55</v>
@@ -2876,31 +2878,31 @@
       <c r="E27" s="9"/>
       <c r="F27" s="6"/>
       <c r="G27" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>56</v>
@@ -2908,10 +2910,10 @@
       <c r="E28" s="9"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
@@ -2919,18 +2921,18 @@
         <v>112</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>57</v>
@@ -2938,31 +2940,31 @@
       <c r="E29" s="9"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>58</v>
@@ -2970,7 +2972,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>113</v>
@@ -2980,21 +2982,21 @@
         <v>92</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>59</v>
@@ -3002,7 +3004,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="6"/>
       <c r="G31" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>114</v>
@@ -3012,21 +3014,21 @@
         <v>93</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>60</v>
@@ -3034,7 +3036,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="6"/>
       <c r="G32" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>115</v>
@@ -3044,21 +3046,21 @@
         <v>93</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>61</v>
@@ -3066,7 +3068,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="6"/>
       <c r="G33" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>116</v>
@@ -3079,18 +3081,18 @@
         <v>112</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>62</v>
@@ -3098,7 +3100,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="6"/>
       <c r="G34" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>117</v>
@@ -3111,18 +3113,18 @@
         <v>112</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>63</v>
@@ -3130,7 +3132,7 @@
       <c r="E35" s="9"/>
       <c r="F35" s="6"/>
       <c r="G35" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>118</v>
@@ -3140,76 +3142,76 @@
         <v>93</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>303</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="6"/>
       <c r="G36" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>81</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="38" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -3220,20 +3222,20 @@
         <v>25</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="6" t="s">
         <v>122</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>91</v>
@@ -3242,10 +3244,10 @@
         <v>93</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -3256,26 +3258,26 @@
         <v>29</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="6"/>
       <c r="G39" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -3286,10 +3288,10 @@
         <v>30</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="6"/>
@@ -3306,47 +3308,47 @@
         <v>81</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="6"/>
       <c r="G41" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I41" s="7"/>
       <c r="J41" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>31</v>
@@ -3355,30 +3357,30 @@
         <v>4</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="6"/>
       <c r="G42" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>32</v>
@@ -3387,25 +3389,25 @@
         <v>4</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="6"/>
       <c r="G43" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -3419,7 +3421,7 @@
         <v>34</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>81</v>
@@ -3429,17 +3431,17 @@
         <v>98</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -3453,153 +3455,153 @@
         <v>36</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>81</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>214</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I46" s="7"/>
       <c r="J46" s="7" t="s">
         <v>81</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="47" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I48" s="7"/>
       <c r="J48" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L48" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7" t="s">
@@ -3609,31 +3611,31 @@
         <v>112</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I50" s="7"/>
       <c r="J50" s="7" t="s">
@@ -3643,31 +3645,31 @@
         <v>112</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7" t="s">
@@ -3677,109 +3679,109 @@
         <v>112</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I52" s="7"/>
       <c r="J52" s="7" t="s">
         <v>81</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="53" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="7" t="s">
         <v>112</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I54" s="11"/>
       <c r="J54" s="7" t="s">
         <v>112</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -3787,23 +3789,23 @@
         <v>103</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>91</v>
@@ -3812,10 +3814,10 @@
         <v>81</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -3823,23 +3825,23 @@
         <v>103</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I56" s="11" t="s">
         <v>91</v>
@@ -3848,10 +3850,10 @@
         <v>81</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="57" spans="1:12" s="4" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -3859,25 +3861,25 @@
         <v>103</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>273</v>
-      </c>
       <c r="E57" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I57" s="11" t="s">
         <v>91</v>
@@ -3886,34 +3888,34 @@
         <v>81</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>284</v>
+        <v>387</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I58" s="11" t="s">
         <v>91</v>
@@ -3922,34 +3924,34 @@
         <v>81</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>284</v>
+        <v>387</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I59" s="7" t="s">
         <v>91</v>
@@ -3958,34 +3960,34 @@
         <v>81</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I60" s="7" t="s">
         <v>91</v>
@@ -3994,34 +3996,34 @@
         <v>81</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F61" s="6"/>
       <c r="G61" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I61" s="7" t="s">
         <v>91</v>
@@ -4030,13 +4032,13 @@
         <v>81</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
         <v>103</v>
       </c>
@@ -4044,17 +4046,17 @@
         <v>38</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>128</v>
@@ -4064,13 +4066,13 @@
         <v>93</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
         <v>103</v>
       </c>
@@ -4078,15 +4080,15 @@
         <v>39</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="6"/>
       <c r="G63" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H63" s="10" t="s">
         <v>128</v>
@@ -4096,13 +4098,13 @@
         <v>93</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
         <v>103</v>
       </c>
@@ -4110,33 +4112,33 @@
         <v>40</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F64" s="6"/>
       <c r="G64" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I64" s="7"/>
       <c r="J64" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
         <v>103</v>
       </c>
@@ -4144,30 +4146,30 @@
         <v>40</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I65" s="7"/>
       <c r="J65" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="1:12" s="4" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -4175,35 +4177,35 @@
         <v>103</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="H66" s="7" t="s">
         <v>249</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>250</v>
       </c>
       <c r="I66" s="7"/>
       <c r="J66" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="67" spans="1:12" s="4" customFormat="1" ht="91" x14ac:dyDescent="0.15">
@@ -4211,25 +4213,25 @@
         <v>103</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>91</v>
@@ -4238,34 +4240,34 @@
         <v>92</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B68" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F68" s="12"/>
       <c r="G68" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>91</v>
@@ -4274,180 +4276,180 @@
         <v>93</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F69" s="12"/>
       <c r="G69" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I69" s="7"/>
       <c r="J69" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F70" s="12"/>
       <c r="G70" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I70" s="7"/>
       <c r="J70" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F71" s="12"/>
       <c r="G71" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I71" s="7"/>
       <c r="J71" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B72" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>264</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F72" s="12"/>
       <c r="G72" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I72" s="7"/>
       <c r="J72" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B73" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>266</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F73" s="12"/>
       <c r="G73" s="7" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I73" s="7"/>
       <c r="J73" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>129</v>
+        <v>387</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -4458,10 +4460,10 @@
         <v>97</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>81</v>
@@ -4483,21 +4485,21 @@
         <v>111</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A75" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>81</v>
@@ -4519,7 +4521,7 @@
         <v>110</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="76" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4530,10 +4532,10 @@
         <v>41</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>81</v>
@@ -4551,7 +4553,7 @@
         <v>110</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="77" spans="1:12" s="4" customFormat="1" ht="221" x14ac:dyDescent="0.15">
@@ -4559,25 +4561,25 @@
         <v>102</v>
       </c>
       <c r="B77" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F77" s="12" t="s">
         <v>285</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F77" s="12" t="s">
-        <v>286</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>98</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -4585,7 +4587,7 @@
         <v>110</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:12" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
@@ -4596,10 +4598,10 @@
         <v>42</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>81</v>
@@ -4609,7 +4611,7 @@
         <v>98</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
@@ -4617,21 +4619,21 @@
         <v>110</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>81</v>
@@ -4641,15 +4643,15 @@
         <v>98</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="80" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4660,10 +4662,10 @@
         <v>108</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>81</v>
@@ -4673,7 +4675,7 @@
         <v>98</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
@@ -4681,7 +4683,7 @@
         <v>110</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4692,10 +4694,10 @@
         <v>109</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>81</v>
@@ -4705,7 +4707,7 @@
         <v>98</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
@@ -4713,7 +4715,7 @@
         <v>110</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4724,10 +4726,10 @@
         <v>37</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="6"/>
@@ -4735,7 +4737,7 @@
         <v>98</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -4743,271 +4745,271 @@
         <v>110</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B83" s="20" t="s">
         <v>43</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E83" s="20" t="s">
         <v>81</v>
       </c>
       <c r="F83" s="21"/>
       <c r="G83" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H83" s="22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I83" s="22"/>
       <c r="J83" s="22" t="s">
         <v>81</v>
       </c>
       <c r="K83" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L83" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="C84" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B84" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="D84" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E84" s="20" t="s">
         <v>82</v>
       </c>
       <c r="F84" s="21"/>
       <c r="G84" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H84" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I84" s="22"/>
       <c r="J84" s="22" t="s">
         <v>92</v>
       </c>
       <c r="K84" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L84" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:12" ht="65" x14ac:dyDescent="0.15">
       <c r="A85" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="C85" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="C85" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="D85" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E85" s="20" t="s">
         <v>81</v>
       </c>
       <c r="F85" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G85" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H85" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I85" s="22"/>
       <c r="J85" s="22" t="s">
         <v>81</v>
       </c>
       <c r="K85" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L85" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C86" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B86" s="20" t="s">
-        <v>316</v>
-      </c>
-      <c r="C86" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="D86" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E86" s="20" t="s">
         <v>81</v>
       </c>
       <c r="F86" s="21"/>
       <c r="G86" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H86" s="22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I86" s="22"/>
       <c r="J86" s="22" t="s">
         <v>81</v>
       </c>
       <c r="K86" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L86" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C87" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B87" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="C87" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="D87" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E87" s="20" t="s">
         <v>93</v>
       </c>
       <c r="F87" s="21"/>
       <c r="G87" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H87" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I87" s="22"/>
       <c r="J87" s="22" t="s">
         <v>93</v>
       </c>
       <c r="K87" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L87" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B88" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="C88" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B88" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="C88" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="D88" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>81</v>
       </c>
       <c r="F88" s="21"/>
       <c r="G88" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H88" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I88" s="22"/>
       <c r="J88" s="22" t="s">
         <v>93</v>
       </c>
       <c r="K88" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L88" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="C89" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B89" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="C89" s="20" t="s">
-        <v>160</v>
-      </c>
       <c r="D89" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>93</v>
       </c>
       <c r="F89" s="21"/>
       <c r="G89" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H89" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I89" s="22"/>
       <c r="J89" s="22" t="s">
         <v>93</v>
       </c>
       <c r="K89" s="22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L89" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="H90" s="7" t="s">
         <v>326</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>327</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>91</v>
@@ -5016,36 +5018,36 @@
         <v>81</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>91</v>
@@ -5054,36 +5056,36 @@
         <v>81</v>
       </c>
       <c r="K91" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G92" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="H92" s="7" t="s">
         <v>326</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>327</v>
       </c>
       <c r="I92" s="7" t="s">
         <v>91</v>
@@ -5092,36 +5094,36 @@
         <v>81</v>
       </c>
       <c r="K92" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A93" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G93" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I93" s="7" t="s">
         <v>91</v>
@@ -5130,68 +5132,68 @@
         <v>81</v>
       </c>
       <c r="K93" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I94" s="7"/>
       <c r="J94" s="7" t="s">
         <v>92</v>
       </c>
       <c r="K94" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I95" s="7" t="s">
         <v>91</v>
@@ -5200,102 +5202,102 @@
         <v>81</v>
       </c>
       <c r="K95" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K96" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>93</v>
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7" t="s">
         <v>93</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C98" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I98" s="7" t="s">
         <v>91</v>
@@ -5304,10 +5306,10 @@
         <v>81</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -5318,28 +5320,28 @@
         <v>45</v>
       </c>
       <c r="C99" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>189</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
       <c r="K99" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L99" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="100" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -5350,28 +5352,28 @@
         <v>46</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="101" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -5382,28 +5384,28 @@
         <v>47</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F101" s="6"/>
       <c r="G101" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="102" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -5414,28 +5416,28 @@
         <v>48</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>92</v>
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -5446,12 +5448,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5706,22 +5712,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5749,12 +5754,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>